<commit_message>
Updated Page object model
</commit_message>
<xml_diff>
--- a/Data/SourceData.xlsx
+++ b/Data/SourceData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\eclipse-workspace\QATasks\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59B3D2B-EB5A-4EA2-B009-7B189AC69E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E043C3-5744-4D63-A88F-4912DBBE2D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Molecule</t>
   </si>
   <si>
+    <t>VANCOMYCIN 1GM</t>
+  </si>
+  <si>
     <t>DOXYCYCLINE 100MG</t>
+  </si>
+  <si>
+    <t>MEROPENEM 1GM</t>
+  </si>
+  <si>
+    <t>CEFTRIAXONE 1GM</t>
+  </si>
+  <si>
+    <t>CLINDAMYCIN 600MG</t>
+  </si>
+  <si>
+    <t>TEICOPLANIN 400MG</t>
+  </si>
+  <si>
+    <t>LINEZOLID 600MG/300ML</t>
+  </si>
+  <si>
+    <t>TIGECYCLINE 50MG</t>
   </si>
 </sst>
 </file>
@@ -363,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -381,7 +402,42 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Molecule - TEICOPLANIN 400MG
</commit_message>
<xml_diff>
--- a/Data/SourceData.xlsx
+++ b/Data/SourceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\eclipse-workspace\QATasks\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E043C3-5744-4D63-A88F-4912DBBE2D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62869DCC-247D-4D0E-A0FB-0D3CD63095E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>